<commit_message>
Manual notes till feb 6th
</commit_message>
<xml_diff>
--- a/Test Case Template.xlsx
+++ b/Test Case Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\009LiveTech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B4072FA-0AF8-4272-BBC3-D84A27F8C911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EF3BD5-CB78-4B19-81F7-D5E4BAA79806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0BF258B6-0441-47D3-980D-A0CAF612A56D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="71">
   <si>
     <t>Project Name</t>
   </si>
@@ -176,6 +176,83 @@
   </si>
   <si>
     <t>app should navigate to "Search Hotel Page"</t>
+  </si>
+  <si>
+    <t>Adactin_Login_TS001_TC002</t>
+  </si>
+  <si>
+    <t>Adactin_Login_TS001_TC003</t>
+  </si>
+  <si>
+    <t>Adactin_Login_TS001_TC004</t>
+  </si>
+  <si>
+    <t>Adactin_Login_TS001_TC005</t>
+  </si>
+  <si>
+    <t>To validdate login using Invalid credentials (Invalid username and valid password)</t>
+  </si>
+  <si>
+    <t>reyaz456</t>
+  </si>
+  <si>
+    <t>Error shoud display below message : 
+"	
+Invalid Login details or Your Password might have expired. Click here to reset your password"</t>
+  </si>
+  <si>
+    <t>To validdate login using Invalid credentials (valid username and Invalid password)</t>
+  </si>
+  <si>
+    <t>reyaz0602</t>
+  </si>
+  <si>
+    <t>To validdate login using Invalid credentials (Invalid username and Invalid password)</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Error should display below text 
+"Enter Username"</t>
+  </si>
+  <si>
+    <t>Adactin_Login_TS001_TC006</t>
+  </si>
+  <si>
+    <t>To validdate login with both username and password  blank fields</t>
+  </si>
+  <si>
+    <t>To validdate login with username and password  blank field</t>
+  </si>
+  <si>
+    <t>Error should display below text 
+"Enter Password"</t>
+  </si>
+  <si>
+    <t>Adactin_Login_TS001_TC007</t>
+  </si>
+  <si>
+    <t>To validdate login with blank username and password  field with data</t>
+  </si>
+  <si>
+    <t>Adactin_Login_TS001_TC008</t>
+  </si>
+  <si>
+    <t>To validdate login with registered username but not verified email</t>
+  </si>
+  <si>
+    <t>user should have registered and not verified his email</t>
+  </si>
+  <si>
+    <t>murthi0602</t>
+  </si>
+  <si>
+    <t>murthi123</t>
+  </si>
+  <si>
+    <t>Error should display below text 
+"Error: Pending Email Verification"</t>
   </si>
 </sst>
 </file>
@@ -592,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FB5A85-1055-4ACD-81B3-2A5F2F033F25}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>
@@ -778,9 +855,489 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="B13" s="5"/>
-      <c r="D13" s="5"/>
+    <row r="13" spans="1:11" ht="117" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="E14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="E15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="E16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="93.6" x14ac:dyDescent="0.45">
+      <c r="E17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="117" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="93.6" x14ac:dyDescent="0.45">
+      <c r="E23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="117" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="93.6" x14ac:dyDescent="0.45">
+      <c r="E29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="93.6" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="46.8" x14ac:dyDescent="0.45">
+      <c r="E33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="70.2" x14ac:dyDescent="0.45">
+      <c r="A35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="46.8" x14ac:dyDescent="0.45">
+      <c r="E38" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="93.6" x14ac:dyDescent="0.45">
+      <c r="A40" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E41" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E42" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="46.8" x14ac:dyDescent="0.45">
+      <c r="E43" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="93.6" x14ac:dyDescent="0.45">
+      <c r="A45" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E46" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E47" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E48" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="5:8" x14ac:dyDescent="0.45">
+      <c r="E49" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="5:8" ht="46.8" x14ac:dyDescent="0.45">
+      <c r="H50" s="5" t="s">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>